<commit_message>
Creando nueva tabla entrada
</commit_message>
<xml_diff>
--- a/htdocs/App/Controllers/HojaEntradaParticulares2017.xlsx
+++ b/htdocs/App/Controllers/HojaEntradaParticulares2017.xlsx
@@ -97,7 +97,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
-    <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="167" formatCode="000\ 00\ 00\ 00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -388,6 +388,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -430,59 +481,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,16 +1298,16 @@
       <c r="Q2" s="26"/>
       <c r="R2" s="26"/>
       <c r="S2" s="26"/>
-      <c r="T2" s="46" t="s">
+      <c r="T2" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="49"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="66"/>
     </row>
     <row r="3" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
@@ -1329,14 +1329,14 @@
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
       <c r="S3" s="14"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="52"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="68"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="69"/>
     </row>
     <row r="4" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
@@ -1348,16 +1348,16 @@
       <c r="G4" s="14"/>
       <c r="R4" s="15"/>
       <c r="S4" s="14"/>
-      <c r="T4" s="45" t="s">
+      <c r="T4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="55"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="72"/>
     </row>
     <row r="5" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
@@ -1369,14 +1369,14 @@
       <c r="G5" s="14"/>
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="58"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="75"/>
     </row>
     <row r="6" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
@@ -1398,16 +1398,16 @@
       <c r="Q6" s="30"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
-      <c r="T6" s="45" t="s">
+      <c r="T6" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="55"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="70"/>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="72"/>
     </row>
     <row r="7" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
@@ -1429,29 +1429,29 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="56"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="57"/>
-      <c r="AA7" s="58"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="75"/>
     </row>
     <row r="8" spans="1:32" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
       <c r="S8" s="13"/>
-      <c r="T8" s="61" t="s">
+      <c r="T8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="59"/>
-      <c r="Y8" s="59"/>
-      <c r="Z8" s="59"/>
-      <c r="AA8" s="59"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="61"/>
+      <c r="AA8" s="61"/>
       <c r="AB8" s="30"/>
       <c r="AC8" s="30"/>
     </row>
@@ -1459,16 +1459,16 @@
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
-      <c r="T9" s="61" t="s">
+      <c r="T9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="54"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="54"/>
+      <c r="AA9" s="54"/>
       <c r="AB9" s="30"/>
       <c r="AC9" s="30"/>
     </row>
@@ -1566,11 +1566,11 @@
       <c r="P13" s="34"/>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
-      <c r="S13" s="63">
+      <c r="S13" s="55">
         <v>0</v>
       </c>
-      <c r="T13" s="63"/>
-      <c r="U13" s="76" t="s">
+      <c r="T13" s="55"/>
+      <c r="U13" s="45" t="s">
         <v>21</v>
       </c>
       <c r="V13" s="33">
@@ -1595,16 +1595,16 @@
       <c r="C14" s="43"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
       <c r="P14" s="34"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
@@ -1638,13 +1638,13 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
-      <c r="S15" s="62" t="s">
+      <c r="S15" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="T15" s="62"/>
-      <c r="U15" s="62"/>
-      <c r="V15" s="62"/>
-      <c r="W15" s="62"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
       <c r="X15" s="35" t="s">
         <v>7</v>
       </c>
@@ -1664,28 +1664,28 @@
         <v>2</v>
       </c>
       <c r="C16" s="44"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="76"/>
+      <c r="O16" s="76"/>
       <c r="P16" s="32"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
-      <c r="S16" s="62" t="s">
+      <c r="S16" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="T16" s="62"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="62"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60"/>
       <c r="X16" s="35" t="s">
         <v>7</v>
       </c>
@@ -1717,13 +1717,13 @@
       <c r="P17" s="34"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
-      <c r="S17" s="62" t="s">
+      <c r="S17" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="60"/>
+      <c r="W17" s="60"/>
       <c r="X17" s="35" t="s">
         <v>7</v>
       </c>
@@ -1742,28 +1742,28 @@
         <v>12</v>
       </c>
       <c r="C18" s="42"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="63"/>
-      <c r="N18" s="63"/>
-      <c r="O18" s="63"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
       <c r="P18" s="34"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
-      <c r="S18" s="62" t="s">
+      <c r="S18" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
       <c r="X18" s="35" t="s">
         <v>7</v>
       </c>
@@ -1794,13 +1794,13 @@
       <c r="P19" s="29"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
-      <c r="S19" s="62" t="s">
+      <c r="S19" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="62"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
       <c r="X19" s="35" t="s">
         <v>7</v>
       </c>
@@ -1831,13 +1831,13 @@
       <c r="P20" s="34"/>
       <c r="Q20" s="14"/>
       <c r="R20" s="14"/>
-      <c r="S20" s="75" t="s">
+      <c r="S20" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
+      <c r="T20" s="60"/>
+      <c r="U20" s="60"/>
+      <c r="V20" s="60"/>
+      <c r="W20" s="60"/>
       <c r="X20" s="36"/>
       <c r="Y20" s="37"/>
       <c r="Z20" s="14"/>
@@ -1851,26 +1851,26 @@
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="63"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
-      <c r="S21" s="75" t="s">
+      <c r="S21" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="T21" s="62"/>
-      <c r="U21" s="62"/>
-      <c r="V21" s="62"/>
-      <c r="W21" s="62"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
       <c r="X21" s="36"/>
       <c r="Y21" s="37"/>
       <c r="Z21" s="14"/>
@@ -1895,11 +1895,11 @@
       <c r="P22" s="34"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14"/>
-      <c r="S22" s="74"/>
-      <c r="T22" s="74"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="74"/>
-      <c r="W22" s="74"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
       <c r="X22" s="36"/>
       <c r="Y22" s="37"/>
       <c r="Z22" s="14"/>
@@ -1911,26 +1911,26 @@
         <v>2</v>
       </c>
       <c r="C23" s="42"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="76"/>
       <c r="P23" s="32"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
       <c r="X23" s="36"/>
       <c r="Y23" s="37"/>
       <c r="Z23" s="14"/>
@@ -1955,11 +1955,11 @@
       <c r="P24" s="34"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
       <c r="X24" s="36"/>
       <c r="Y24" s="37"/>
       <c r="Z24" s="14"/>
@@ -1967,30 +1967,30 @@
     </row>
     <row r="25" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="31"/>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="71"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
       <c r="P25" s="38"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
       <c r="X25" s="36"/>
       <c r="Y25" s="37"/>
       <c r="Z25" s="14"/>
@@ -2016,11 +2016,11 @@
       <c r="P26" s="29"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
       <c r="X26" s="36"/>
       <c r="Y26" s="37"/>
       <c r="Z26" s="14"/>
@@ -2046,11 +2046,11 @@
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
-      <c r="S27" s="64"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="W27" s="64"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
       <c r="X27" s="36"/>
       <c r="Y27" s="37"/>
       <c r="Z27" s="14"/>
@@ -2059,11 +2059,11 @@
     </row>
     <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R28" s="14"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="64"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
       <c r="X28" s="36"/>
       <c r="Y28" s="37"/>
       <c r="Z28" s="14"/>
@@ -2071,11 +2071,11 @@
     </row>
     <row r="29" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R29" s="14"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="60"/>
-      <c r="U29" s="60"/>
-      <c r="V29" s="60"/>
-      <c r="W29" s="60"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="54"/>
+      <c r="W29" s="54"/>
       <c r="X29" s="39" t="s">
         <v>7</v>
       </c>
@@ -2085,11 +2085,11 @@
     </row>
     <row r="30" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R30" s="14"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="60"/>
-      <c r="U30" s="60"/>
-      <c r="V30" s="60"/>
-      <c r="W30" s="60"/>
+      <c r="S30" s="54"/>
+      <c r="T30" s="54"/>
+      <c r="U30" s="54"/>
+      <c r="V30" s="54"/>
+      <c r="W30" s="54"/>
       <c r="X30" s="39" t="s">
         <v>7</v>
       </c>
@@ -2159,20 +2159,20 @@
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
-      <c r="S33" s="73" t="s">
+      <c r="S33" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="T33" s="73"/>
-      <c r="U33" s="73"/>
-      <c r="V33" s="73"/>
-      <c r="W33" s="73"/>
-      <c r="X33" s="65">
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="47">
         <f>SUM(Y15:Y30)</f>
         <v>121</v>
       </c>
-      <c r="Y33" s="66"/>
-      <c r="Z33" s="66"/>
-      <c r="AA33" s="67"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="48"/>
+      <c r="AA33" s="49"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
@@ -2193,15 +2193,15 @@
       <c r="P34" s="14"/>
       <c r="Q34" s="30"/>
       <c r="R34" s="12"/>
-      <c r="S34" s="73"/>
-      <c r="T34" s="73"/>
-      <c r="U34" s="73"/>
-      <c r="V34" s="73"/>
-      <c r="W34" s="73"/>
-      <c r="X34" s="68"/>
-      <c r="Y34" s="69"/>
-      <c r="Z34" s="69"/>
-      <c r="AA34" s="70"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56"/>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="51"/>
+      <c r="Z34" s="51"/>
+      <c r="AA34" s="52"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
@@ -2417,6 +2417,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="T4:W5"/>
+    <mergeCell ref="T2:W3"/>
+    <mergeCell ref="T6:W7"/>
+    <mergeCell ref="X2:AA3"/>
+    <mergeCell ref="X4:AA5"/>
+    <mergeCell ref="X6:AA7"/>
+    <mergeCell ref="X8:AA8"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="S16:W16"/>
+    <mergeCell ref="S15:W15"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S18:W18"/>
+    <mergeCell ref="S17:W17"/>
+    <mergeCell ref="S29:W29"/>
+    <mergeCell ref="S28:W28"/>
+    <mergeCell ref="S27:W27"/>
+    <mergeCell ref="S26:W26"/>
+    <mergeCell ref="S25:W25"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="X33:AA34"/>
     <mergeCell ref="D25:O25"/>
@@ -2433,26 +2453,6 @@
     <mergeCell ref="S21:W21"/>
     <mergeCell ref="S20:W20"/>
     <mergeCell ref="S19:W19"/>
-    <mergeCell ref="S18:W18"/>
-    <mergeCell ref="S17:W17"/>
-    <mergeCell ref="S29:W29"/>
-    <mergeCell ref="S28:W28"/>
-    <mergeCell ref="S27:W27"/>
-    <mergeCell ref="S26:W26"/>
-    <mergeCell ref="S25:W25"/>
-    <mergeCell ref="X8:AA8"/>
-    <mergeCell ref="X9:AA9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="S16:W16"/>
-    <mergeCell ref="S15:W15"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="T4:W5"/>
-    <mergeCell ref="T2:W3"/>
-    <mergeCell ref="T6:W7"/>
-    <mergeCell ref="X2:AA3"/>
-    <mergeCell ref="X4:AA5"/>
-    <mergeCell ref="X6:AA7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.35433070866141736" right="0.15748031496062992" top="0.2" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>